<commit_message>
Tüm Python dosyaları güncellendi
</commit_message>
<xml_diff>
--- a/data/bundesliga_final_dataset.xlsx
+++ b/data/bundesliga_final_dataset.xlsx
@@ -502,31 +502,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>1.75</v>
+        <v>1.6</v>
       </c>
       <c r="D2" t="n">
-        <v>3.7</v>
+        <v>4.5</v>
       </c>
       <c r="E2" t="n">
-        <v>3.7</v>
+        <v>4.5</v>
       </c>
       <c r="F2" t="n">
-        <v>6.4</v>
+        <v>7.9</v>
       </c>
       <c r="G2" t="n">
-        <v>0.92</v>
+        <v>0.89</v>
       </c>
       <c r="H2" t="n">
-        <v>1.59</v>
+        <v>1.58</v>
       </c>
       <c r="I2" t="n">
-        <v>0.92</v>
+        <v>0.89</v>
       </c>
       <c r="J2" t="n">
-        <v>1.59</v>
+        <v>1.58</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -582,31 +582,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>2.25</v>
+        <v>2.2</v>
       </c>
       <c r="D4" t="n">
-        <v>7.8</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>8.4</v>
       </c>
       <c r="F4" t="n">
-        <v>13.1</v>
+        <v>15.8</v>
       </c>
       <c r="G4" t="n">
-        <v>1.95</v>
+        <v>1.84</v>
       </c>
       <c r="H4" t="n">
-        <v>3.46</v>
+        <v>3.33</v>
       </c>
       <c r="I4" t="n">
-        <v>1.75</v>
+        <v>1.69</v>
       </c>
       <c r="J4" t="n">
-        <v>3.26</v>
+        <v>3.17</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -622,31 +622,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C5" t="n">
-        <v>2.75</v>
+        <v>3.4</v>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>6.2</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
-        <v>11.9</v>
+        <v>17.2</v>
       </c>
       <c r="G5" t="n">
-        <v>1.75</v>
+        <v>1.96</v>
       </c>
       <c r="H5" t="n">
-        <v>3.17</v>
+        <v>3.6</v>
       </c>
       <c r="I5" t="n">
-        <v>1.55</v>
+        <v>1.8</v>
       </c>
       <c r="J5" t="n">
-        <v>2.98</v>
+        <v>3.44</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
@@ -662,31 +662,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>1.75</v>
+        <v>1.6</v>
       </c>
       <c r="D6" t="n">
-        <v>7.3</v>
+        <v>8.5</v>
       </c>
       <c r="E6" t="n">
-        <v>4.9</v>
+        <v>6.1</v>
       </c>
       <c r="F6" t="n">
-        <v>9.1</v>
+        <v>11.4</v>
       </c>
       <c r="G6" t="n">
-        <v>1.82</v>
+        <v>1.69</v>
       </c>
       <c r="H6" t="n">
-        <v>2.86</v>
+        <v>2.76</v>
       </c>
       <c r="I6" t="n">
-        <v>1.23</v>
+        <v>1.22</v>
       </c>
       <c r="J6" t="n">
-        <v>2.27</v>
+        <v>2.29</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -702,31 +702,31 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
         <v>1</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.25</v>
-      </c>
       <c r="D7" t="n">
-        <v>5.2</v>
+        <v>6.9</v>
       </c>
       <c r="E7" t="n">
-        <v>5.2</v>
+        <v>6.9</v>
       </c>
       <c r="F7" t="n">
-        <v>9.1</v>
+        <v>12</v>
       </c>
       <c r="G7" t="n">
-        <v>1.3</v>
+        <v>1.37</v>
       </c>
       <c r="H7" t="n">
-        <v>2.28</v>
+        <v>2.41</v>
       </c>
       <c r="I7" t="n">
-        <v>1.3</v>
+        <v>1.37</v>
       </c>
       <c r="J7" t="n">
-        <v>2.28</v>
+        <v>2.41</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -745,28 +745,28 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D8" t="n">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="E8" t="n">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="F8" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G8" t="n">
-        <v>0.86</v>
+        <v>0.9</v>
       </c>
       <c r="H8" t="n">
-        <v>1.51</v>
+        <v>1.6</v>
       </c>
       <c r="I8" t="n">
-        <v>0.86</v>
+        <v>0.9</v>
       </c>
       <c r="J8" t="n">
-        <v>1.51</v>
+        <v>1.6</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -782,31 +782,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>6.2</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>6.2</v>
       </c>
       <c r="F9" t="n">
-        <v>9.4</v>
+        <v>11.5</v>
       </c>
       <c r="G9" t="n">
-        <v>1.25</v>
+        <v>1.24</v>
       </c>
       <c r="H9" t="n">
-        <v>2.35</v>
+        <v>2.3</v>
       </c>
       <c r="I9" t="n">
-        <v>1.25</v>
+        <v>1.24</v>
       </c>
       <c r="J9" t="n">
-        <v>2.35</v>
+        <v>2.3</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
@@ -822,31 +822,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="D10" t="n">
-        <v>5.4</v>
+        <v>7.9</v>
       </c>
       <c r="E10" t="n">
-        <v>3.8</v>
+        <v>6.3</v>
       </c>
       <c r="F10" t="n">
-        <v>6.8</v>
+        <v>11.5</v>
       </c>
       <c r="G10" t="n">
-        <v>1.35</v>
+        <v>1.57</v>
       </c>
       <c r="H10" t="n">
-        <v>2.1</v>
+        <v>2.62</v>
       </c>
       <c r="I10" t="n">
-        <v>0.96</v>
+        <v>1.26</v>
       </c>
       <c r="J10" t="n">
-        <v>1.71</v>
+        <v>2.31</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -862,31 +862,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>6.8</v>
+        <v>7.9</v>
       </c>
       <c r="E11" t="n">
-        <v>6.8</v>
+        <v>7.9</v>
       </c>
       <c r="F11" t="n">
-        <v>12.4</v>
+        <v>14.3</v>
       </c>
       <c r="G11" t="n">
-        <v>1.7</v>
+        <v>1.57</v>
       </c>
       <c r="H11" t="n">
-        <v>3.09</v>
+        <v>2.86</v>
       </c>
       <c r="I11" t="n">
-        <v>1.7</v>
+        <v>1.57</v>
       </c>
       <c r="J11" t="n">
-        <v>3.09</v>
+        <v>2.86</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
@@ -902,31 +902,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C12" t="n">
         <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>6.3</v>
+        <v>7.2</v>
       </c>
       <c r="E12" t="n">
-        <v>4.7</v>
+        <v>5.6</v>
       </c>
       <c r="F12" t="n">
-        <v>8.199999999999999</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="G12" t="n">
-        <v>1.58</v>
+        <v>1.44</v>
       </c>
       <c r="H12" t="n">
-        <v>2.44</v>
+        <v>2.26</v>
       </c>
       <c r="I12" t="n">
-        <v>1.18</v>
+        <v>1.12</v>
       </c>
       <c r="J12" t="n">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="K12" t="n">
         <v>0</v>
@@ -945,28 +945,28 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>7</v>
+        <v>7.4</v>
       </c>
       <c r="E13" t="n">
-        <v>6.2</v>
+        <v>6.7</v>
       </c>
       <c r="F13" t="n">
-        <v>10.8</v>
+        <v>11.7</v>
       </c>
       <c r="G13" t="n">
-        <v>1.74</v>
+        <v>1.49</v>
       </c>
       <c r="H13" t="n">
-        <v>2.9</v>
+        <v>2.51</v>
       </c>
       <c r="I13" t="n">
-        <v>1.55</v>
+        <v>1.33</v>
       </c>
       <c r="J13" t="n">
-        <v>2.7</v>
+        <v>2.35</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -982,31 +982,31 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="D14" t="n">
-        <v>7.8</v>
+        <v>10</v>
       </c>
       <c r="E14" t="n">
-        <v>7.8</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="F14" t="n">
-        <v>12.5</v>
+        <v>14.7</v>
       </c>
       <c r="G14" t="n">
-        <v>1.95</v>
+        <v>2.01</v>
       </c>
       <c r="H14" t="n">
         <v>3.11</v>
       </c>
       <c r="I14" t="n">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="J14" t="n">
-        <v>3.11</v>
+        <v>2.95</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
@@ -1022,31 +1022,31 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" t="n">
-        <v>1.75</v>
+        <v>1.6</v>
       </c>
       <c r="D15" t="n">
-        <v>5.4</v>
+        <v>6.2</v>
       </c>
       <c r="E15" t="n">
-        <v>3.8</v>
+        <v>4.6</v>
       </c>
       <c r="F15" t="n">
-        <v>6.6</v>
+        <v>8</v>
       </c>
       <c r="G15" t="n">
-        <v>1.36</v>
+        <v>1.25</v>
       </c>
       <c r="H15" t="n">
-        <v>2.04</v>
+        <v>1.93</v>
       </c>
       <c r="I15" t="n">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="J15" t="n">
-        <v>1.64</v>
+        <v>1.61</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
@@ -1062,31 +1062,31 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C16" t="n">
-        <v>1.25</v>
+        <v>1.4</v>
       </c>
       <c r="D16" t="n">
-        <v>5</v>
+        <v>6.9</v>
       </c>
       <c r="E16" t="n">
-        <v>4.2</v>
+        <v>5.3</v>
       </c>
       <c r="F16" t="n">
-        <v>8.1</v>
+        <v>10.2</v>
       </c>
       <c r="G16" t="n">
-        <v>1.26</v>
+        <v>1.38</v>
       </c>
       <c r="H16" t="n">
-        <v>2.23</v>
+        <v>2.35</v>
       </c>
       <c r="I16" t="n">
         <v>1.06</v>
       </c>
       <c r="J16" t="n">
-        <v>2.03</v>
+        <v>2.04</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
@@ -1105,28 +1105,28 @@
         <v>8</v>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="D17" t="n">
-        <v>5.7</v>
+        <v>7</v>
       </c>
       <c r="E17" t="n">
-        <v>5.7</v>
+        <v>6.3</v>
       </c>
       <c r="F17" t="n">
-        <v>9.300000000000001</v>
+        <v>10.2</v>
       </c>
       <c r="G17" t="n">
-        <v>1.42</v>
+        <v>1.41</v>
       </c>
       <c r="H17" t="n">
-        <v>2.33</v>
+        <v>2.2</v>
       </c>
       <c r="I17" t="n">
-        <v>1.42</v>
+        <v>1.25</v>
       </c>
       <c r="J17" t="n">
-        <v>2.33</v>
+        <v>2.04</v>
       </c>
       <c r="K17" t="n">
         <v>0</v>
@@ -1185,28 +1185,28 @@
         <v>7</v>
       </c>
       <c r="C19" t="n">
-        <v>1.75</v>
+        <v>1.4</v>
       </c>
       <c r="D19" t="n">
-        <v>5.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E19" t="n">
-        <v>4.5</v>
+        <v>7.5</v>
       </c>
       <c r="F19" t="n">
-        <v>8.300000000000001</v>
+        <v>13.9</v>
       </c>
       <c r="G19" t="n">
-        <v>1.33</v>
+        <v>1.66</v>
       </c>
       <c r="H19" t="n">
-        <v>2.28</v>
+        <v>2.93</v>
       </c>
       <c r="I19" t="n">
-        <v>1.13</v>
+        <v>1.5</v>
       </c>
       <c r="J19" t="n">
-        <v>2.08</v>
+        <v>2.77</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
🧠 Son güncellemeler eklendi
</commit_message>
<xml_diff>
--- a/data/bundesliga_final_dataset.xlsx
+++ b/data/bundesliga_final_dataset.xlsx
@@ -502,31 +502,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" t="n">
-        <v>1.6</v>
+        <v>1.83</v>
       </c>
       <c r="D2" t="n">
-        <v>4.5</v>
+        <v>6.3</v>
       </c>
       <c r="E2" t="n">
-        <v>4.5</v>
+        <v>6.3</v>
       </c>
       <c r="F2" t="n">
-        <v>7.9</v>
+        <v>11.5</v>
       </c>
       <c r="G2" t="n">
-        <v>0.89</v>
+        <v>1.05</v>
       </c>
       <c r="H2" t="n">
-        <v>1.58</v>
+        <v>1.92</v>
       </c>
       <c r="I2" t="n">
-        <v>0.89</v>
+        <v>1.05</v>
       </c>
       <c r="J2" t="n">
-        <v>1.58</v>
+        <v>1.92</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -542,31 +542,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>4.4</v>
+        <v>4.17</v>
       </c>
       <c r="D3" t="n">
-        <v>14.7</v>
+        <v>16.4</v>
       </c>
       <c r="E3" t="n">
-        <v>11.7</v>
+        <v>13.4</v>
       </c>
       <c r="F3" t="n">
-        <v>21.3</v>
+        <v>24.4</v>
       </c>
       <c r="G3" t="n">
-        <v>2.94</v>
+        <v>2.73</v>
       </c>
       <c r="H3" t="n">
-        <v>4.86</v>
+        <v>4.57</v>
       </c>
       <c r="I3" t="n">
-        <v>2.34</v>
+        <v>2.23</v>
       </c>
       <c r="J3" t="n">
-        <v>4.26</v>
+        <v>4.07</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -582,31 +582,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>2.2</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>9.199999999999999</v>
+        <v>10.1</v>
       </c>
       <c r="E4" t="n">
-        <v>8.4</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>15.8</v>
+        <v>17.5</v>
       </c>
       <c r="G4" t="n">
-        <v>1.84</v>
+        <v>1.68</v>
       </c>
       <c r="H4" t="n">
-        <v>3.33</v>
+        <v>3.04</v>
       </c>
       <c r="I4" t="n">
-        <v>1.69</v>
+        <v>1.55</v>
       </c>
       <c r="J4" t="n">
-        <v>3.17</v>
+        <v>2.91</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -625,28 +625,28 @@
         <v>17</v>
       </c>
       <c r="C5" t="n">
-        <v>3.4</v>
+        <v>2.83</v>
       </c>
       <c r="D5" t="n">
-        <v>9.800000000000001</v>
+        <v>10.1</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="F5" t="n">
-        <v>17.2</v>
+        <v>17.6</v>
       </c>
       <c r="G5" t="n">
-        <v>1.96</v>
+        <v>1.68</v>
       </c>
       <c r="H5" t="n">
-        <v>3.6</v>
+        <v>3.07</v>
       </c>
       <c r="I5" t="n">
-        <v>1.8</v>
+        <v>1.55</v>
       </c>
       <c r="J5" t="n">
-        <v>3.44</v>
+        <v>2.94</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
@@ -665,28 +665,28 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>1.6</v>
+        <v>1.33</v>
       </c>
       <c r="D6" t="n">
-        <v>8.5</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E6" t="n">
-        <v>6.1</v>
+        <v>6.8</v>
       </c>
       <c r="F6" t="n">
-        <v>11.4</v>
+        <v>12.5</v>
       </c>
       <c r="G6" t="n">
-        <v>1.69</v>
+        <v>1.53</v>
       </c>
       <c r="H6" t="n">
-        <v>2.76</v>
+        <v>2.47</v>
       </c>
       <c r="I6" t="n">
-        <v>1.22</v>
+        <v>1.13</v>
       </c>
       <c r="J6" t="n">
-        <v>2.29</v>
+        <v>2.08</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -705,28 +705,28 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="D7" t="n">
-        <v>6.9</v>
+        <v>7.4</v>
       </c>
       <c r="E7" t="n">
-        <v>6.9</v>
+        <v>7.4</v>
       </c>
       <c r="F7" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G7" t="n">
-        <v>1.37</v>
+        <v>1.23</v>
       </c>
       <c r="H7" t="n">
-        <v>2.41</v>
+        <v>2.17</v>
       </c>
       <c r="I7" t="n">
-        <v>1.37</v>
+        <v>1.23</v>
       </c>
       <c r="J7" t="n">
-        <v>2.41</v>
+        <v>2.17</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -742,37 +742,37 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>4.5</v>
+        <v>6.4</v>
       </c>
       <c r="E8" t="n">
-        <v>4.5</v>
+        <v>6.4</v>
       </c>
       <c r="F8" t="n">
-        <v>8</v>
+        <v>11.4</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9</v>
+        <v>1.07</v>
       </c>
       <c r="H8" t="n">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9</v>
+        <v>1.07</v>
       </c>
       <c r="J8" t="n">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>1</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="9">
@@ -785,28 +785,28 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8</v>
+        <v>0.67</v>
       </c>
       <c r="D9" t="n">
-        <v>6.2</v>
+        <v>6.8</v>
       </c>
       <c r="E9" t="n">
-        <v>6.2</v>
+        <v>6.8</v>
       </c>
       <c r="F9" t="n">
-        <v>11.5</v>
+        <v>12.6</v>
       </c>
       <c r="G9" t="n">
-        <v>1.24</v>
+        <v>1.13</v>
       </c>
       <c r="H9" t="n">
-        <v>2.3</v>
+        <v>2.09</v>
       </c>
       <c r="I9" t="n">
-        <v>1.24</v>
+        <v>1.13</v>
       </c>
       <c r="J9" t="n">
-        <v>2.3</v>
+        <v>2.09</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
@@ -825,28 +825,28 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="D10" t="n">
-        <v>7.9</v>
+        <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>6.3</v>
+        <v>7.4</v>
       </c>
       <c r="F10" t="n">
-        <v>11.5</v>
+        <v>13.6</v>
       </c>
       <c r="G10" t="n">
-        <v>1.57</v>
+        <v>1.5</v>
       </c>
       <c r="H10" t="n">
-        <v>2.62</v>
+        <v>2.54</v>
       </c>
       <c r="I10" t="n">
-        <v>1.26</v>
+        <v>1.23</v>
       </c>
       <c r="J10" t="n">
-        <v>2.31</v>
+        <v>2.27</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -862,31 +862,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="D11" t="n">
-        <v>7.9</v>
+        <v>9</v>
       </c>
       <c r="E11" t="n">
-        <v>7.9</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
-        <v>14.3</v>
+        <v>16.6</v>
       </c>
       <c r="G11" t="n">
-        <v>1.57</v>
+        <v>1.51</v>
       </c>
       <c r="H11" t="n">
-        <v>2.86</v>
+        <v>2.76</v>
       </c>
       <c r="I11" t="n">
-        <v>1.57</v>
+        <v>1.51</v>
       </c>
       <c r="J11" t="n">
-        <v>2.86</v>
+        <v>2.76</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
@@ -902,31 +902,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C12" t="n">
         <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>7.2</v>
+        <v>10.1</v>
       </c>
       <c r="E12" t="n">
-        <v>5.6</v>
+        <v>8.5</v>
       </c>
       <c r="F12" t="n">
-        <v>9.699999999999999</v>
+        <v>13.8</v>
       </c>
       <c r="G12" t="n">
-        <v>1.44</v>
+        <v>1.68</v>
       </c>
       <c r="H12" t="n">
-        <v>2.26</v>
+        <v>2.57</v>
       </c>
       <c r="I12" t="n">
-        <v>1.12</v>
+        <v>1.42</v>
       </c>
       <c r="J12" t="n">
-        <v>1.95</v>
+        <v>2.3</v>
       </c>
       <c r="K12" t="n">
         <v>0</v>
@@ -945,28 +945,28 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="D13" t="n">
-        <v>7.4</v>
+        <v>8.1</v>
       </c>
       <c r="E13" t="n">
-        <v>6.7</v>
+        <v>7.3</v>
       </c>
       <c r="F13" t="n">
-        <v>11.7</v>
+        <v>13</v>
       </c>
       <c r="G13" t="n">
-        <v>1.49</v>
+        <v>1.35</v>
       </c>
       <c r="H13" t="n">
-        <v>2.51</v>
+        <v>2.3</v>
       </c>
       <c r="I13" t="n">
-        <v>1.33</v>
+        <v>1.22</v>
       </c>
       <c r="J13" t="n">
-        <v>2.35</v>
+        <v>2.16</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -982,37 +982,37 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>1.4</v>
+        <v>1.33</v>
       </c>
       <c r="D14" t="n">
-        <v>10</v>
+        <v>11.1</v>
       </c>
       <c r="E14" t="n">
-        <v>9.199999999999999</v>
+        <v>10.4</v>
       </c>
       <c r="F14" t="n">
-        <v>14.7</v>
+        <v>16.7</v>
       </c>
       <c r="G14" t="n">
-        <v>2.01</v>
+        <v>1.86</v>
       </c>
       <c r="H14" t="n">
-        <v>3.11</v>
+        <v>2.92</v>
       </c>
       <c r="I14" t="n">
-        <v>1.85</v>
+        <v>1.73</v>
       </c>
       <c r="J14" t="n">
-        <v>2.95</v>
+        <v>2.78</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="15">
@@ -1025,28 +1025,28 @@
         <v>8</v>
       </c>
       <c r="C15" t="n">
-        <v>1.6</v>
+        <v>1.33</v>
       </c>
       <c r="D15" t="n">
-        <v>6.2</v>
+        <v>7</v>
       </c>
       <c r="E15" t="n">
-        <v>4.6</v>
+        <v>5.4</v>
       </c>
       <c r="F15" t="n">
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="G15" t="n">
-        <v>1.25</v>
+        <v>1.16</v>
       </c>
       <c r="H15" t="n">
-        <v>1.93</v>
+        <v>1.85</v>
       </c>
       <c r="I15" t="n">
-        <v>0.93</v>
+        <v>0.9</v>
       </c>
       <c r="J15" t="n">
-        <v>1.61</v>
+        <v>1.58</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
@@ -1062,31 +1062,31 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C16" t="n">
-        <v>1.4</v>
+        <v>1.33</v>
       </c>
       <c r="D16" t="n">
-        <v>6.9</v>
+        <v>7.9</v>
       </c>
       <c r="E16" t="n">
-        <v>5.3</v>
+        <v>6.3</v>
       </c>
       <c r="F16" t="n">
-        <v>10.2</v>
+        <v>12</v>
       </c>
       <c r="G16" t="n">
-        <v>1.38</v>
+        <v>1.31</v>
       </c>
       <c r="H16" t="n">
-        <v>2.35</v>
+        <v>2.26</v>
       </c>
       <c r="I16" t="n">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
       <c r="J16" t="n">
-        <v>2.04</v>
+        <v>1.99</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
@@ -1105,28 +1105,28 @@
         <v>8</v>
       </c>
       <c r="C17" t="n">
-        <v>1.6</v>
+        <v>1.33</v>
       </c>
       <c r="D17" t="n">
-        <v>7</v>
+        <v>7.9</v>
       </c>
       <c r="E17" t="n">
-        <v>6.3</v>
+        <v>7.1</v>
       </c>
       <c r="F17" t="n">
-        <v>10.2</v>
+        <v>11.9</v>
       </c>
       <c r="G17" t="n">
-        <v>1.41</v>
+        <v>1.32</v>
       </c>
       <c r="H17" t="n">
-        <v>2.2</v>
+        <v>2.11</v>
       </c>
       <c r="I17" t="n">
-        <v>1.25</v>
+        <v>1.18</v>
       </c>
       <c r="J17" t="n">
-        <v>2.04</v>
+        <v>1.98</v>
       </c>
       <c r="K17" t="n">
         <v>0</v>
@@ -1142,31 +1142,31 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C18" t="n">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="D18" t="n">
-        <v>6.8</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="E18" t="n">
-        <v>4.5</v>
+        <v>6.3</v>
       </c>
       <c r="F18" t="n">
-        <v>8.4</v>
+        <v>11.6</v>
       </c>
       <c r="G18" t="n">
-        <v>1.36</v>
+        <v>1.44</v>
       </c>
       <c r="H18" t="n">
-        <v>2.15</v>
+        <v>2.32</v>
       </c>
       <c r="I18" t="n">
-        <v>0.9</v>
+        <v>1.06</v>
       </c>
       <c r="J18" t="n">
-        <v>1.69</v>
+        <v>1.93</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
@@ -1182,31 +1182,31 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>1.4</v>
+        <v>1.33</v>
       </c>
       <c r="D19" t="n">
-        <v>8.300000000000001</v>
+        <v>9.5</v>
       </c>
       <c r="E19" t="n">
-        <v>7.5</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="F19" t="n">
-        <v>13.9</v>
+        <v>16.2</v>
       </c>
       <c r="G19" t="n">
-        <v>1.66</v>
+        <v>1.58</v>
       </c>
       <c r="H19" t="n">
-        <v>2.93</v>
+        <v>2.83</v>
       </c>
       <c r="I19" t="n">
-        <v>1.5</v>
+        <v>1.45</v>
       </c>
       <c r="J19" t="n">
-        <v>2.77</v>
+        <v>2.69</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Tüm dosyalar güncellendi - son model, veri ve app.py dahil
</commit_message>
<xml_diff>
--- a/data/bundesliga_final_dataset.xlsx
+++ b/data/bundesliga_final_dataset.xlsx
@@ -505,28 +505,28 @@
         <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>1.71</v>
+        <v>1.5</v>
       </c>
       <c r="D2" t="n">
-        <v>7.4</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>6.7</v>
+        <v>7.5</v>
       </c>
       <c r="F2" t="n">
-        <v>12.1</v>
+        <v>13.5</v>
       </c>
       <c r="G2" t="n">
-        <v>1.06</v>
+        <v>1.03</v>
       </c>
       <c r="H2" t="n">
-        <v>1.84</v>
+        <v>1.79</v>
       </c>
       <c r="I2" t="n">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="J2" t="n">
-        <v>1.73</v>
+        <v>1.69</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -542,31 +542,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>3.86</v>
+        <v>3.75</v>
       </c>
       <c r="D3" t="n">
-        <v>18.8</v>
+        <v>22.8</v>
       </c>
       <c r="E3" t="n">
-        <v>15.8</v>
+        <v>19.8</v>
       </c>
       <c r="F3" t="n">
-        <v>28.3</v>
+        <v>35.7</v>
       </c>
       <c r="G3" t="n">
-        <v>2.69</v>
+        <v>2.85</v>
       </c>
       <c r="H3" t="n">
-        <v>4.47</v>
+        <v>4.84</v>
       </c>
       <c r="I3" t="n">
-        <v>2.26</v>
+        <v>2.47</v>
       </c>
       <c r="J3" t="n">
-        <v>4.05</v>
+        <v>4.46</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -582,31 +582,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="n">
-        <v>1.86</v>
+        <v>1.75</v>
       </c>
       <c r="D4" t="n">
-        <v>11.7</v>
+        <v>13.6</v>
       </c>
       <c r="E4" t="n">
-        <v>10.9</v>
+        <v>12.8</v>
       </c>
       <c r="F4" t="n">
-        <v>20.4</v>
+        <v>24.1</v>
       </c>
       <c r="G4" t="n">
-        <v>1.67</v>
+        <v>1.69</v>
       </c>
       <c r="H4" t="n">
-        <v>3.03</v>
+        <v>3.11</v>
       </c>
       <c r="I4" t="n">
-        <v>1.56</v>
+        <v>1.6</v>
       </c>
       <c r="J4" t="n">
-        <v>2.91</v>
+        <v>3.01</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -622,31 +622,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5" t="n">
-        <v>2.71</v>
+        <v>2.62</v>
       </c>
       <c r="D5" t="n">
-        <v>10.9</v>
+        <v>13.1</v>
       </c>
       <c r="E5" t="n">
-        <v>10.1</v>
+        <v>12.3</v>
       </c>
       <c r="F5" t="n">
-        <v>18.9</v>
+        <v>22.6</v>
       </c>
       <c r="G5" t="n">
-        <v>1.55</v>
+        <v>1.64</v>
       </c>
       <c r="H5" t="n">
-        <v>2.81</v>
+        <v>2.92</v>
       </c>
       <c r="I5" t="n">
-        <v>1.44</v>
+        <v>1.54</v>
       </c>
       <c r="J5" t="n">
-        <v>2.69</v>
+        <v>2.82</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
@@ -665,28 +665,28 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>1.43</v>
+        <v>1.25</v>
       </c>
       <c r="D6" t="n">
-        <v>10.3</v>
+        <v>10.9</v>
       </c>
       <c r="E6" t="n">
-        <v>7.9</v>
+        <v>8.5</v>
       </c>
       <c r="F6" t="n">
-        <v>14.6</v>
+        <v>15.6</v>
       </c>
       <c r="G6" t="n">
-        <v>1.47</v>
+        <v>1.36</v>
       </c>
       <c r="H6" t="n">
-        <v>2.42</v>
+        <v>2.25</v>
       </c>
       <c r="I6" t="n">
-        <v>1.13</v>
+        <v>1.07</v>
       </c>
       <c r="J6" t="n">
-        <v>2.08</v>
+        <v>1.96</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -705,10 +705,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0.86</v>
+        <v>0.75</v>
       </c>
       <c r="D7" t="n">
-        <v>8.1</v>
+        <v>8.9</v>
       </c>
       <c r="E7" t="n">
         <v>8.1</v>
@@ -717,16 +717,16 @@
         <v>14.5</v>
       </c>
       <c r="G7" t="n">
-        <v>1.16</v>
+        <v>1.11</v>
       </c>
       <c r="H7" t="n">
-        <v>2.07</v>
+        <v>1.91</v>
       </c>
       <c r="I7" t="n">
-        <v>1.16</v>
+        <v>1.02</v>
       </c>
       <c r="J7" t="n">
-        <v>2.07</v>
+        <v>1.81</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -745,28 +745,28 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0.87</v>
       </c>
       <c r="D8" t="n">
-        <v>7.9</v>
+        <v>10.7</v>
       </c>
       <c r="E8" t="n">
-        <v>7.9</v>
+        <v>9.9</v>
       </c>
       <c r="F8" t="n">
-        <v>14.3</v>
+        <v>17.8</v>
       </c>
       <c r="G8" t="n">
-        <v>1.13</v>
+        <v>1.34</v>
       </c>
       <c r="H8" t="n">
-        <v>2.05</v>
+        <v>2.32</v>
       </c>
       <c r="I8" t="n">
-        <v>1.13</v>
+        <v>1.24</v>
       </c>
       <c r="J8" t="n">
-        <v>2.05</v>
+        <v>2.22</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -782,31 +782,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>0.86</v>
+        <v>0.87</v>
       </c>
       <c r="D9" t="n">
-        <v>9.6</v>
+        <v>11.1</v>
       </c>
       <c r="E9" t="n">
-        <v>9.6</v>
+        <v>11.1</v>
       </c>
       <c r="F9" t="n">
-        <v>17.4</v>
+        <v>20.5</v>
       </c>
       <c r="G9" t="n">
-        <v>1.37</v>
+        <v>1.39</v>
       </c>
       <c r="H9" t="n">
-        <v>2.49</v>
+        <v>2.56</v>
       </c>
       <c r="I9" t="n">
-        <v>1.37</v>
+        <v>1.39</v>
       </c>
       <c r="J9" t="n">
-        <v>2.49</v>
+        <v>2.56</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
@@ -822,31 +822,31 @@
         </is>
       </c>
       <c r="B10" t="n">
+        <v>15</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="D10" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="E10" t="n">
         <v>12</v>
       </c>
-      <c r="C10" t="n">
-        <v>1.71</v>
-      </c>
-      <c r="D10" t="n">
-        <v>11.3</v>
-      </c>
-      <c r="E10" t="n">
-        <v>9.699999999999999</v>
-      </c>
       <c r="F10" t="n">
-        <v>18.3</v>
+        <v>22.6</v>
       </c>
       <c r="G10" t="n">
-        <v>1.62</v>
+        <v>1.7</v>
       </c>
       <c r="H10" t="n">
+        <v>3.02</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="J10" t="n">
         <v>2.83</v>
-      </c>
-      <c r="I10" t="n">
-        <v>1.39</v>
-      </c>
-      <c r="J10" t="n">
-        <v>2.61</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -865,28 +865,28 @@
         <v>12</v>
       </c>
       <c r="C11" t="n">
-        <v>1.71</v>
+        <v>1.5</v>
       </c>
       <c r="D11" t="n">
-        <v>9.6</v>
+        <v>10.1</v>
       </c>
       <c r="E11" t="n">
-        <v>9.6</v>
+        <v>10.1</v>
       </c>
       <c r="F11" t="n">
-        <v>17.5</v>
+        <v>18.4</v>
       </c>
       <c r="G11" t="n">
-        <v>1.37</v>
+        <v>1.27</v>
       </c>
       <c r="H11" t="n">
-        <v>2.5</v>
+        <v>2.3</v>
       </c>
       <c r="I11" t="n">
-        <v>1.37</v>
+        <v>1.27</v>
       </c>
       <c r="J11" t="n">
-        <v>2.5</v>
+        <v>2.3</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
@@ -902,31 +902,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C12" t="n">
-        <v>2.29</v>
+        <v>2.25</v>
       </c>
       <c r="D12" t="n">
-        <v>13.4</v>
+        <v>15.1</v>
       </c>
       <c r="E12" t="n">
-        <v>11.1</v>
+        <v>12.8</v>
       </c>
       <c r="F12" t="n">
-        <v>18.7</v>
+        <v>21.5</v>
       </c>
       <c r="G12" t="n">
-        <v>1.92</v>
+        <v>1.89</v>
       </c>
       <c r="H12" t="n">
-        <v>3</v>
+        <v>2.98</v>
       </c>
       <c r="I12" t="n">
-        <v>1.59</v>
+        <v>1.6</v>
       </c>
       <c r="J12" t="n">
-        <v>2.67</v>
+        <v>2.69</v>
       </c>
       <c r="K12" t="n">
         <v>0</v>
@@ -942,31 +942,31 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" t="n">
-        <v>1.14</v>
+        <v>1.13</v>
       </c>
       <c r="D13" t="n">
-        <v>9.699999999999999</v>
+        <v>11.1</v>
       </c>
       <c r="E13" t="n">
-        <v>8.199999999999999</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="F13" t="n">
-        <v>14.3</v>
+        <v>15.4</v>
       </c>
       <c r="G13" t="n">
         <v>1.39</v>
       </c>
       <c r="H13" t="n">
-        <v>2.27</v>
+        <v>2.21</v>
       </c>
       <c r="I13" t="n">
-        <v>1.17</v>
+        <v>1.1</v>
       </c>
       <c r="J13" t="n">
-        <v>2.05</v>
+        <v>1.92</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -982,31 +982,31 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C14" t="n">
-        <v>1.43</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>12.4</v>
+        <v>15.1</v>
       </c>
       <c r="E14" t="n">
-        <v>11.6</v>
+        <v>14.3</v>
       </c>
       <c r="F14" t="n">
-        <v>19.1</v>
+        <v>23.9</v>
       </c>
       <c r="G14" t="n">
-        <v>1.77</v>
+        <v>1.89</v>
       </c>
       <c r="H14" t="n">
-        <v>2.85</v>
+        <v>3.09</v>
       </c>
       <c r="I14" t="n">
-        <v>1.66</v>
+        <v>1.79</v>
       </c>
       <c r="J14" t="n">
-        <v>2.74</v>
+        <v>2.99</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
@@ -1025,28 +1025,28 @@
         <v>8</v>
       </c>
       <c r="C15" t="n">
-        <v>1.14</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>7.9</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>6.3</v>
+        <v>6.7</v>
       </c>
       <c r="F15" t="n">
-        <v>11.2</v>
+        <v>11.8</v>
       </c>
       <c r="G15" t="n">
-        <v>1.13</v>
+        <v>1.04</v>
       </c>
       <c r="H15" t="n">
-        <v>1.83</v>
+        <v>1.68</v>
       </c>
       <c r="I15" t="n">
-        <v>0.9</v>
+        <v>0.84</v>
       </c>
       <c r="J15" t="n">
-        <v>1.6</v>
+        <v>1.47</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
@@ -1062,31 +1062,31 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C16" t="n">
-        <v>1.57</v>
+        <v>1.62</v>
       </c>
       <c r="D16" t="n">
-        <v>9.699999999999999</v>
+        <v>11.6</v>
       </c>
       <c r="E16" t="n">
-        <v>8.1</v>
+        <v>10.1</v>
       </c>
       <c r="F16" t="n">
-        <v>15.5</v>
+        <v>18.6</v>
       </c>
       <c r="G16" t="n">
-        <v>1.39</v>
+        <v>1.45</v>
       </c>
       <c r="H16" t="n">
-        <v>2.44</v>
+        <v>2.53</v>
       </c>
       <c r="I16" t="n">
-        <v>1.16</v>
+        <v>1.26</v>
       </c>
       <c r="J16" t="n">
-        <v>2.22</v>
+        <v>2.33</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
@@ -1105,28 +1105,28 @@
         <v>11</v>
       </c>
       <c r="C17" t="n">
-        <v>1.57</v>
+        <v>1.37</v>
       </c>
       <c r="D17" t="n">
-        <v>9.1</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>8.300000000000001</v>
+        <v>8.9</v>
       </c>
       <c r="F17" t="n">
-        <v>13.7</v>
+        <v>14.8</v>
       </c>
       <c r="G17" t="n">
-        <v>1.3</v>
+        <v>1.21</v>
       </c>
       <c r="H17" t="n">
-        <v>2.07</v>
+        <v>1.95</v>
       </c>
       <c r="I17" t="n">
-        <v>1.19</v>
+        <v>1.11</v>
       </c>
       <c r="J17" t="n">
-        <v>1.96</v>
+        <v>1.85</v>
       </c>
       <c r="K17" t="n">
         <v>0</v>
@@ -1142,31 +1142,31 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" t="n">
-        <v>1.57</v>
+        <v>1.5</v>
       </c>
       <c r="D18" t="n">
-        <v>9.699999999999999</v>
+        <v>11.1</v>
       </c>
       <c r="E18" t="n">
-        <v>7.4</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="F18" t="n">
-        <v>13.5</v>
+        <v>15.7</v>
       </c>
       <c r="G18" t="n">
-        <v>1.39</v>
+        <v>1.38</v>
       </c>
       <c r="H18" t="n">
-        <v>2.26</v>
+        <v>2.25</v>
       </c>
       <c r="I18" t="n">
-        <v>1.06</v>
+        <v>1.09</v>
       </c>
       <c r="J18" t="n">
-        <v>1.92</v>
+        <v>1.96</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
@@ -1182,31 +1182,31 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C19" t="n">
-        <v>1.14</v>
+        <v>1.13</v>
       </c>
       <c r="D19" t="n">
-        <v>9.9</v>
+        <v>10.3</v>
       </c>
       <c r="E19" t="n">
-        <v>9.199999999999999</v>
+        <v>9.5</v>
       </c>
       <c r="F19" t="n">
-        <v>16.9</v>
+        <v>17.7</v>
       </c>
       <c r="G19" t="n">
-        <v>1.42</v>
+        <v>1.29</v>
       </c>
       <c r="H19" t="n">
-        <v>2.53</v>
+        <v>2.31</v>
       </c>
       <c r="I19" t="n">
-        <v>1.31</v>
+        <v>1.19</v>
       </c>
       <c r="J19" t="n">
-        <v>2.42</v>
+        <v>2.21</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>

</xml_diff>